<commit_message>
Schematic (Minus Connectors) Complete
</commit_message>
<xml_diff>
--- a/hardware/parts/BOM.xlsx
+++ b/hardware/parts/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mois\Documents\GitHub\Mercury\hardware\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C0176B-4EFC-45FB-95FD-30CBBCBF8C86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0C5AC0-F85F-4370-AF55-1EC9738F944A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{20CA75D0-32CF-46D3-AED3-BC8C3487575F}"/>
+    <workbookView xWindow="11028" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{20CA75D0-32CF-46D3-AED3-BC8C3487575F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>Comment</t>
   </si>
@@ -56,15 +56,6 @@
     <t>MFR. Part #</t>
   </si>
   <si>
-    <t>STM32H743IIT6</t>
-  </si>
-  <si>
-    <t>LQFP-176_24.0x24.0x0.5P</t>
-  </si>
-  <si>
-    <t>C89597</t>
-  </si>
-  <si>
     <t>Main MCU</t>
   </si>
   <si>
@@ -167,12 +158,6 @@
     <t>LQFP-100_14.0x14.0x0.5P</t>
   </si>
   <si>
-    <t>Main MCU ALT</t>
-  </si>
-  <si>
-    <t>REMOVE</t>
-  </si>
-  <si>
     <t>STM32F407VGT6</t>
   </si>
   <si>
@@ -225,6 +210,21 @@
   </si>
   <si>
     <t>SMA Connector</t>
+  </si>
+  <si>
+    <t>KDS Daishinku</t>
+  </si>
+  <si>
+    <t>1C/N226000AA0D</t>
+  </si>
+  <si>
+    <t>SMD-3225_4P</t>
+  </si>
+  <si>
+    <t>C160424</t>
+  </si>
+  <si>
+    <t>26 MHz Oscillator</t>
   </si>
 </sst>
 </file>
@@ -626,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A664FD-7BBB-46C5-962E-B53DC8A09416}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +637,7 @@
     <col min="1" max="7" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -648,7 +648,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -660,203 +660,200 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>41</v>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="B12" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="4"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
         <v>51</v>
@@ -868,32 +865,29 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>54</v>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://lcsc.com/product-detail/ST-Microelectronics_STMicroelectronics_STM32H743IIT6_STM32H743IIT6_C89597.html/?href=jlc-SMT" xr:uid="{BBDBB47D-E704-4840-9261-22A1B6365041}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>